<commit_message>
added more functionality and UI + selectedHero is first one (Zho)
</commit_message>
<xml_diff>
--- a/Documents/Calculations.xlsx
+++ b/Documents/Calculations.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Upgrades" sheetId="1" r:id="rId1"/>
+    <sheet name="Damage" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
   <si>
     <t>Zhouyu</t>
   </si>
@@ -47,24 +47,15 @@
     <t>Lvl 3</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Lvl 4</t>
   </si>
   <si>
     <t>Lvl 5</t>
   </si>
   <si>
-    <t>Damage\Levels</t>
-  </si>
-  <si>
     <t>Tap Cost\Levels</t>
   </si>
   <si>
-    <t>Heros Cost\Levels</t>
-  </si>
-  <si>
     <t>Tap Damage\Levels</t>
   </si>
   <si>
@@ -92,16 +83,7 @@
     <t>Buff Duration (sec)\Levels</t>
   </si>
   <si>
-    <t>Enemy Health\ Levels</t>
-  </si>
-  <si>
-    <t>Balloon</t>
-  </si>
-  <si>
-    <t>Zeppelin</t>
-  </si>
-  <si>
-    <t>Enemy Damage\ Levels</t>
+    <t xml:space="preserve">Heros </t>
   </si>
 </sst>
 </file>
@@ -166,28 +148,7 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="49">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -349,25 +310,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C2:H6" totalsRowShown="0" headerRowDxfId="49" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C2:H6" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="C2:H6"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Heros Cost\Levels"/>
-    <tableColumn id="2" name="Lvl 1" dataDxfId="55"/>
-    <tableColumn id="3" name="Lvl 2" dataDxfId="54"/>
-    <tableColumn id="4" name="Lvl 3" dataDxfId="53"/>
-    <tableColumn id="5" name="Lvl 4" dataDxfId="52"/>
-    <tableColumn id="6" name="Lvl 5" dataDxfId="51"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C8:H12" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="C8:H12"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Damage\Levels"/>
+    <tableColumn id="1" name="Heros "/>
     <tableColumn id="2" name="Lvl 1" dataDxfId="46"/>
     <tableColumn id="3" name="Lvl 2" dataDxfId="45"/>
     <tableColumn id="4" name="Lvl 3" dataDxfId="44"/>
@@ -378,9 +324,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="C16:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="C16:H17"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="C11:H12" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="C11:H12"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Tap Cost\Levels"/>
     <tableColumn id="2" name="Lvl 1" dataDxfId="39" dataCellStyle="Bad"/>
@@ -393,9 +339,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1378" displayName="Table1378" ref="C19:H20" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="C19:H20"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1378" displayName="Table1378" ref="C14:H15" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="C14:H15"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Tap Damage\Levels"/>
     <tableColumn id="2" name="Lvl 1" dataDxfId="32" dataCellStyle="Bad"/>
@@ -408,9 +354,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table13710" displayName="Table13710" ref="C24:H25" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="C24:H25"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table13710" displayName="Table13710" ref="C19:H20" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="C19:H20"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Ability Cost\Levels"/>
     <tableColumn id="2" name="Lvl 1" dataDxfId="25" dataCellStyle="Bad"/>
@@ -423,9 +369,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1371011" displayName="Table1371011" ref="C27:H28" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="C27:H28"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1371011" displayName="Table1371011" ref="C22:H23" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="C22:H23"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Ability Damage\Levels"/>
     <tableColumn id="2" name="Lvl 1" dataDxfId="18"/>
@@ -438,9 +384,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1371012" displayName="Table1371012" ref="C32:H34" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="C32:H34"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1371012" displayName="Table1371012" ref="C27:H29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="C27:H29"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Buff Cost\Levels"/>
     <tableColumn id="2" name="Lvl 1" dataDxfId="11" dataCellStyle="Bad"/>
@@ -453,9 +399,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table137101213" displayName="Table137101213" ref="C36:H38" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="C36:H38"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table137101213" displayName="Table137101213" ref="C31:H33" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="C31:H33"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Buff Duration (sec)\Levels"/>
     <tableColumn id="2" name="Lvl 1" dataDxfId="4" dataCellStyle="Bad"/>
@@ -731,23 +677,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:P38"/>
+  <dimension ref="C2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="9.140625" style="1"/>
-    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
     <col min="12" max="16" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -759,295 +705,208 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+      <c r="D3" s="1">
+        <v>10</v>
       </c>
       <c r="E3" s="1">
-        <v>200</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1">
-        <v>400</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1">
-        <v>800</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>1200</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
-        <v>1800</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1">
-        <v>2200</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1">
-        <v>2600</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1">
-        <v>3000</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>5000</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1">
-        <v>6200</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1">
-        <v>7400</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1">
-        <v>8500</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1">
-        <v>9600</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>10000</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1">
-        <v>12000</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1">
-        <v>14000</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1">
-        <v>16000</v>
+        <v>46</v>
       </c>
       <c r="H6" s="1">
-        <v>1800</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1">
-        <v>20</v>
-      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>50</v>
-      </c>
-      <c r="E10" s="1">
-        <v>60</v>
-      </c>
-      <c r="F10" s="1">
-        <v>80</v>
-      </c>
-      <c r="G10" s="1">
-        <v>100</v>
-      </c>
-      <c r="H10" s="1">
-        <v>150</v>
-      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>200</v>
-      </c>
-      <c r="E11" s="1">
-        <v>220</v>
-      </c>
-      <c r="F11" s="1">
-        <v>240</v>
-      </c>
-      <c r="G11" s="1">
-        <v>280</v>
-      </c>
-      <c r="H11" s="1">
-        <v>340</v>
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1">
-        <v>500</v>
-      </c>
-      <c r="E12" s="1">
-        <v>600</v>
-      </c>
-      <c r="F12" s="1">
-        <v>700</v>
-      </c>
-      <c r="G12" s="1">
-        <v>850</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>4</v>
@@ -1059,15 +918,15 @@
         <v>6</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1075,35 +934,45 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="1" t="s">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1">
         <v>16</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="F23" s="1">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1">
+        <v>24</v>
+      </c>
+      <c r="H23" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
@@ -1119,55 +988,65 @@
         <v>6</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="1">
-        <v>10</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="1">
-        <v>20</v>
-      </c>
-      <c r="G28" s="1">
-        <v>24</v>
-      </c>
-      <c r="H28" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="3" t="s">
-        <v>19</v>
+      <c r="C33" t="s">
+        <v>17</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1175,59 +1054,9 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="8">
+  <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -1235,7 +1064,6 @@
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>